<commit_message>
Xong thị trường tất cả
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportDetailtByPartner.xlsx
+++ b/DongAERP/Content/Report/ReportDetailtByPartner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DongAERP\DongAERP\DongAERP\Content\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FC5D0-72E6-4A6E-99CA-EABB6211B40E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B844D84-6495-40AE-A01D-7A2EEF3F9F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Từ:</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>GBP</t>
-  </si>
-  <si>
-    <t>Tổng quy USD</t>
   </si>
 </sst>
 </file>
@@ -172,17 +169,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B6D35-F82E-4989-A479-5B01F28891A5}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,29 +510,29 @@
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="22.21875" customWidth="1"/>
     <col min="8" max="8" width="23.88671875" customWidth="1"/>
-    <col min="9" max="9" width="26.5546875" customWidth="1"/>
-    <col min="15" max="15" width="18.5546875" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="18.5546875" customWidth="1"/>
-    <col min="19" max="19" width="18.5546875" style="1" customWidth="1"/>
-    <col min="20" max="21" width="18.6640625" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" style="1" customWidth="1"/>
+    <col min="19" max="20" width="18.6640625" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
@@ -545,19 +542,18 @@
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -567,123 +563,118 @@
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="5"/>
-    </row>
-    <row r="7" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="T6" s="6"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O25" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>